<commit_message>
Adding Easv5 and Dasv5 SAPs as per July update on SAP NOTE 1928533
</commit_message>
<xml_diff>
--- a/SAPs.xlsx
+++ b/SAPs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10627"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10710"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abicas/Documents/dev/SAP CALC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD540AC-51EE-6448-8821-8F7B667DA64F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8306BC-110E-8D4B-8BF2-B6A2A1EDB3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="3160" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{45FA4414-BA71-AA46-A273-049CCFF9F681}"/>
+    <workbookView xWindow="4560" yWindow="3160" windowWidth="27640" windowHeight="16940" xr2:uid="{45FA4414-BA71-AA46-A273-049CCFF9F681}"/>
   </bookViews>
   <sheets>
     <sheet name="SAPs" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="129">
   <si>
     <t>E2as v4</t>
   </si>
@@ -396,6 +396,57 @@
   </si>
   <si>
     <t>BR South (USD)</t>
+  </si>
+  <si>
+    <t>D2as v5</t>
+  </si>
+  <si>
+    <t>D4as v5</t>
+  </si>
+  <si>
+    <t>D8as v5</t>
+  </si>
+  <si>
+    <t>D16as v5</t>
+  </si>
+  <si>
+    <t>D32as v5</t>
+  </si>
+  <si>
+    <t>D48as v5</t>
+  </si>
+  <si>
+    <t>D64as v5</t>
+  </si>
+  <si>
+    <t>D96as v5</t>
+  </si>
+  <si>
+    <t>E2as v5</t>
+  </si>
+  <si>
+    <t>E4as v5</t>
+  </si>
+  <si>
+    <t>E8as v5</t>
+  </si>
+  <si>
+    <t>E16as v5</t>
+  </si>
+  <si>
+    <t>E20as v5</t>
+  </si>
+  <si>
+    <t>E32as v5</t>
+  </si>
+  <si>
+    <t>E48as v5</t>
+  </si>
+  <si>
+    <t>E64as v5</t>
+  </si>
+  <si>
+    <t>E96as v5</t>
   </si>
 </sst>
 </file>
@@ -509,19 +560,19 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -837,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{697A7A29-3B64-0E4E-BF4A-313D8DB48D19}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1989,16 +2040,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="B68">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="C68">
-        <v>512</v>
+        <v>8</v>
       </c>
       <c r="D68">
-        <v>66600</v>
+        <v>3070</v>
       </c>
       <c r="E68" t="s">
         <v>14</v>
@@ -2006,188 +2057,477 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="B69">
-        <v>208</v>
+        <v>4</v>
       </c>
       <c r="C69">
-        <v>2850</v>
+        <v>16</v>
       </c>
       <c r="D69">
-        <v>259950</v>
+        <v>6140</v>
       </c>
       <c r="E69" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="B70">
-        <v>208</v>
+        <v>8</v>
       </c>
       <c r="C70">
-        <v>5700</v>
+        <v>32</v>
       </c>
       <c r="D70">
-        <v>259950</v>
+        <v>12281</v>
       </c>
       <c r="E70" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="B71">
-        <v>4126</v>
+        <v>16</v>
       </c>
       <c r="C71">
-        <v>5700</v>
+        <v>64</v>
       </c>
       <c r="D71">
-        <v>488230</v>
+        <v>25562</v>
       </c>
       <c r="E71" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="B72">
-        <v>416</v>
+        <v>32</v>
       </c>
       <c r="C72">
-        <v>11400</v>
+        <v>128</v>
       </c>
       <c r="D72">
-        <v>488230</v>
+        <v>49123</v>
       </c>
       <c r="E72" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="B73">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C73">
-        <v>875</v>
+        <v>192</v>
       </c>
       <c r="D73">
-        <v>42711</v>
+        <v>73685</v>
       </c>
       <c r="E73" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="B74">
         <v>64</v>
       </c>
       <c r="C74">
-        <v>1024</v>
+        <v>256</v>
       </c>
       <c r="D74">
-        <v>85432</v>
+        <v>98247</v>
       </c>
       <c r="E74" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
       <c r="B75">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="C75">
-        <v>1792</v>
+        <v>384</v>
       </c>
       <c r="D75">
-        <v>85432</v>
+        <v>147370</v>
       </c>
       <c r="E75" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="B76">
-        <v>128</v>
+        <v>2</v>
       </c>
       <c r="C76">
-        <v>2048</v>
+        <v>16</v>
       </c>
       <c r="D76">
-        <v>170846</v>
+        <v>3070</v>
       </c>
       <c r="E76" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="B77">
-        <v>128</v>
+        <v>4</v>
       </c>
       <c r="C77">
-        <v>4096</v>
+        <v>32</v>
       </c>
       <c r="D77">
-        <v>170846</v>
+        <v>6140</v>
       </c>
       <c r="E77" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="B78">
-        <v>192</v>
+        <v>8</v>
       </c>
       <c r="C78">
-        <v>2048</v>
+        <v>64</v>
       </c>
       <c r="D78">
-        <v>256750</v>
+        <v>12281</v>
       </c>
       <c r="E78" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>123</v>
+      </c>
+      <c r="B79">
+        <v>16</v>
+      </c>
+      <c r="C79">
+        <v>128</v>
+      </c>
+      <c r="D79">
+        <v>24562</v>
+      </c>
+      <c r="E79" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>124</v>
+      </c>
+      <c r="B80">
+        <v>20</v>
+      </c>
+      <c r="C80">
+        <v>160</v>
+      </c>
+      <c r="D80">
+        <v>30702</v>
+      </c>
+      <c r="E80" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>125</v>
+      </c>
+      <c r="B81">
+        <v>32</v>
+      </c>
+      <c r="C81">
+        <v>256</v>
+      </c>
+      <c r="D81">
+        <v>49123</v>
+      </c>
+      <c r="E81" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>126</v>
+      </c>
+      <c r="B82">
+        <v>48</v>
+      </c>
+      <c r="C82">
+        <v>384</v>
+      </c>
+      <c r="D82">
+        <v>73685</v>
+      </c>
+      <c r="E82" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>127</v>
+      </c>
+      <c r="B83">
+        <v>64</v>
+      </c>
+      <c r="C83">
+        <v>512</v>
+      </c>
+      <c r="D83">
+        <v>98247</v>
+      </c>
+      <c r="E83" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>128</v>
+      </c>
+      <c r="B84">
+        <v>96</v>
+      </c>
+      <c r="C84">
+        <v>672</v>
+      </c>
+      <c r="D84">
+        <v>147370</v>
+      </c>
+      <c r="E84" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>72</v>
+      </c>
+      <c r="B85">
+        <v>64</v>
+      </c>
+      <c r="C85">
+        <v>512</v>
+      </c>
+      <c r="D85">
+        <v>66600</v>
+      </c>
+      <c r="E85" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>208</v>
+      </c>
+      <c r="C86">
+        <v>2850</v>
+      </c>
+      <c r="D86">
+        <v>259950</v>
+      </c>
+      <c r="E86" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>208</v>
+      </c>
+      <c r="C87">
+        <v>5700</v>
+      </c>
+      <c r="D87">
+        <v>259950</v>
+      </c>
+      <c r="E87" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>4126</v>
+      </c>
+      <c r="C88">
+        <v>5700</v>
+      </c>
+      <c r="D88">
+        <v>488230</v>
+      </c>
+      <c r="E88" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>416</v>
+      </c>
+      <c r="C89">
+        <v>11400</v>
+      </c>
+      <c r="D89">
+        <v>488230</v>
+      </c>
+      <c r="E89" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>78</v>
+      </c>
+      <c r="B90">
+        <v>32</v>
+      </c>
+      <c r="C90">
+        <v>875</v>
+      </c>
+      <c r="D90">
+        <v>42711</v>
+      </c>
+      <c r="E90" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>79</v>
+      </c>
+      <c r="B91">
+        <v>64</v>
+      </c>
+      <c r="C91">
+        <v>1024</v>
+      </c>
+      <c r="D91">
+        <v>85432</v>
+      </c>
+      <c r="E91" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>80</v>
+      </c>
+      <c r="B92">
+        <v>64</v>
+      </c>
+      <c r="C92">
+        <v>1792</v>
+      </c>
+      <c r="D92">
+        <v>85432</v>
+      </c>
+      <c r="E92" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>81</v>
+      </c>
+      <c r="B93">
+        <v>128</v>
+      </c>
+      <c r="C93">
+        <v>2048</v>
+      </c>
+      <c r="D93">
+        <v>170846</v>
+      </c>
+      <c r="E93" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>82</v>
+      </c>
+      <c r="B94">
+        <v>128</v>
+      </c>
+      <c r="C94">
+        <v>4096</v>
+      </c>
+      <c r="D94">
+        <v>170846</v>
+      </c>
+      <c r="E94" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>83</v>
+      </c>
+      <c r="B95">
+        <v>192</v>
+      </c>
+      <c r="C95">
+        <v>2048</v>
+      </c>
+      <c r="D95">
+        <v>256750</v>
+      </c>
+      <c r="E95" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>84</v>
       </c>
-      <c r="B79">
+      <c r="B96">
         <v>192</v>
       </c>
-      <c r="C79">
+      <c r="C96">
         <v>4096</v>
       </c>
-      <c r="D79">
+      <c r="D96">
         <v>256750</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E96" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2201,7 +2541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D48ADED-64D6-E94C-BADE-AF9BDA6012C6}">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -2333,384 +2673,69 @@
       <c r="H16"/>
       <c r="I16"/>
     </row>
-    <row r="17" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-    </row>
-    <row r="18" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
-    </row>
-    <row r="19" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
-    </row>
-    <row r="20" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-    </row>
-    <row r="21" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
-    </row>
-    <row r="22" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-    </row>
-    <row r="23" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
-    </row>
-    <row r="24" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
-    </row>
-    <row r="25" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25"/>
-      <c r="I25"/>
-    </row>
-    <row r="26" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F26"/>
-      <c r="G26"/>
-      <c r="H26"/>
-      <c r="I26"/>
-    </row>
-    <row r="27" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F27"/>
-      <c r="G27"/>
-      <c r="H27"/>
-      <c r="I27"/>
-    </row>
-    <row r="28" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28"/>
-    </row>
-    <row r="29" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
-    </row>
-    <row r="30" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30"/>
-      <c r="I30"/>
-    </row>
-    <row r="31" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31"/>
-    </row>
-    <row r="32" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32"/>
-    </row>
-    <row r="33" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
-    </row>
-    <row r="34" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F34"/>
-      <c r="G34"/>
-      <c r="H34"/>
-      <c r="I34"/>
-    </row>
-    <row r="35" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35"/>
-      <c r="I35"/>
-    </row>
-    <row r="36" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F36"/>
-      <c r="G36"/>
-      <c r="H36"/>
-      <c r="I36"/>
-    </row>
-    <row r="37" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F37"/>
-      <c r="G37"/>
-      <c r="H37"/>
-      <c r="I37"/>
-    </row>
-    <row r="38" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F38"/>
-      <c r="G38"/>
-      <c r="H38"/>
-      <c r="I38"/>
-    </row>
-    <row r="39" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F39"/>
-      <c r="G39"/>
-      <c r="H39"/>
-      <c r="I39"/>
-    </row>
-    <row r="40" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40"/>
-      <c r="I40"/>
-    </row>
-    <row r="41" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F41"/>
-      <c r="G41"/>
-      <c r="H41"/>
-      <c r="I41"/>
-    </row>
-    <row r="42" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F42"/>
-      <c r="G42"/>
-      <c r="H42"/>
-      <c r="I42"/>
-    </row>
-    <row r="43" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F43"/>
-      <c r="G43"/>
-      <c r="H43"/>
-      <c r="I43"/>
-    </row>
-    <row r="44" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F44"/>
-      <c r="G44"/>
-      <c r="H44"/>
-      <c r="I44"/>
-    </row>
-    <row r="45" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F45"/>
-      <c r="G45"/>
-      <c r="H45"/>
-      <c r="I45"/>
-    </row>
-    <row r="46" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F46"/>
-      <c r="G46"/>
-      <c r="H46"/>
-      <c r="I46"/>
-    </row>
-    <row r="47" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F47"/>
-      <c r="G47"/>
-      <c r="H47"/>
-      <c r="I47"/>
-    </row>
-    <row r="48" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F48"/>
-      <c r="G48"/>
-      <c r="H48"/>
-      <c r="I48"/>
-    </row>
-    <row r="49" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F49"/>
-      <c r="G49"/>
-      <c r="H49"/>
-      <c r="I49"/>
-    </row>
-    <row r="50" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F50"/>
-      <c r="G50"/>
-      <c r="H50"/>
-      <c r="I50"/>
-    </row>
-    <row r="51" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F51"/>
-      <c r="G51"/>
-      <c r="H51"/>
-      <c r="I51"/>
-    </row>
-    <row r="52" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F52"/>
-      <c r="G52"/>
-      <c r="H52"/>
-      <c r="I52"/>
-    </row>
-    <row r="53" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F53"/>
-      <c r="G53"/>
-      <c r="H53"/>
-      <c r="I53"/>
-    </row>
-    <row r="54" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F54"/>
-      <c r="G54"/>
-      <c r="H54"/>
-      <c r="I54"/>
-    </row>
-    <row r="55" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F55"/>
-      <c r="G55"/>
-      <c r="H55"/>
-      <c r="I55"/>
-    </row>
-    <row r="56" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F56"/>
-      <c r="G56"/>
-      <c r="H56"/>
-      <c r="I56"/>
-    </row>
-    <row r="57" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F57"/>
-      <c r="G57"/>
-      <c r="H57"/>
-      <c r="I57"/>
-    </row>
-    <row r="58" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F58"/>
-      <c r="G58"/>
-      <c r="H58"/>
-      <c r="I58"/>
-    </row>
-    <row r="59" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F59"/>
-      <c r="G59"/>
-      <c r="H59"/>
-      <c r="I59"/>
-    </row>
-    <row r="60" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F60"/>
-      <c r="G60"/>
-      <c r="H60"/>
-      <c r="I60"/>
-    </row>
-    <row r="61" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F61"/>
-      <c r="G61"/>
-      <c r="H61"/>
-      <c r="I61"/>
-    </row>
-    <row r="62" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F62"/>
-      <c r="G62"/>
-      <c r="H62"/>
-      <c r="I62"/>
-    </row>
-    <row r="63" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F63"/>
-      <c r="G63"/>
-      <c r="H63"/>
-      <c r="I63"/>
-    </row>
-    <row r="64" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F64"/>
-      <c r="G64"/>
-      <c r="H64"/>
-      <c r="I64"/>
-    </row>
-    <row r="65" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F65"/>
-      <c r="G65"/>
-      <c r="H65"/>
-      <c r="I65"/>
-    </row>
-    <row r="66" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F66"/>
-      <c r="G66"/>
-      <c r="H66"/>
-      <c r="I66"/>
-    </row>
-    <row r="67" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F67"/>
-      <c r="G67"/>
-      <c r="H67"/>
-      <c r="I67"/>
-    </row>
-    <row r="68" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F68"/>
-      <c r="G68"/>
-      <c r="H68"/>
-      <c r="I68"/>
-    </row>
-    <row r="69" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F69"/>
-      <c r="G69"/>
-      <c r="H69"/>
-      <c r="I69"/>
-    </row>
-    <row r="70" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F70"/>
-      <c r="G70"/>
-      <c r="H70"/>
-      <c r="I70"/>
-    </row>
-    <row r="71" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F71"/>
-      <c r="G71"/>
-      <c r="H71"/>
-      <c r="I71"/>
-    </row>
-    <row r="72" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F72"/>
-      <c r="G72"/>
-      <c r="H72"/>
-      <c r="I72"/>
-    </row>
-    <row r="73" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F73"/>
-      <c r="G73"/>
-      <c r="H73"/>
-      <c r="I73"/>
-    </row>
-    <row r="74" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F74"/>
-      <c r="G74"/>
-      <c r="H74"/>
-      <c r="I74"/>
-    </row>
-    <row r="75" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F75"/>
-      <c r="G75"/>
-      <c r="H75"/>
-      <c r="I75"/>
-    </row>
-    <row r="76" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F76"/>
-      <c r="G76"/>
-      <c r="H76"/>
-      <c r="I76"/>
-    </row>
-    <row r="77" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F77"/>
-      <c r="G77"/>
-      <c r="H77"/>
-      <c r="I77"/>
-    </row>
-    <row r="78" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F78"/>
-      <c r="G78"/>
-      <c r="H78"/>
-      <c r="I78"/>
-    </row>
-    <row r="79" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F79"/>
-      <c r="G79"/>
-      <c r="H79"/>
-      <c r="I79"/>
-    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="48" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2721,7 +2746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687EF088-C94A-FB47-9F82-811747A0B89F}">
   <dimension ref="A1:T80"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
@@ -2735,35 +2760,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="J1" s="13" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="J1" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13" t="s">
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13" t="s">
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="R1" s="13"/>
+      <c r="R1" s="14"/>
       <c r="S1" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="T1" s="14"/>
+      <c r="T1" s="16"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -2867,19 +2892,19 @@
         <f t="array" ref="N3">IF(NOT(ISNA($T3)),INDEX(Pricelist!D$2:D$150,$T3),)</f>
         <v>0</v>
       </c>
-      <c r="O3" s="16" cm="1">
+      <c r="O3" s="13" cm="1">
         <f t="array" ref="O3">IF(NOT(ISNA($T3)),INDEX(Pricelist!F$2:F$150,$T3),)</f>
         <v>0</v>
       </c>
-      <c r="P3" s="16" cm="1">
+      <c r="P3" s="13" cm="1">
         <f t="array" ref="P3">IF(NOT(ISNA($T3)),INDEX(Pricelist!G$2:G$150,$T3),)</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="16" cm="1">
+      <c r="Q3" s="13" cm="1">
         <f t="array" ref="Q3">IF(NOT(ISNA($T3)),INDEX(Pricelist!H$2:H$150,$T3),)</f>
         <v>0</v>
       </c>
-      <c r="R3" s="16" cm="1">
+      <c r="R3" s="13" cm="1">
         <f t="array" ref="R3">IF(NOT(ISNA($T3)),INDEX(Pricelist!I$2:I$150,$T3),)</f>
         <v>0</v>
       </c>
@@ -2935,19 +2960,19 @@
         <f t="array" ref="N4">IF(NOT(ISNA($T4)),INDEX(Pricelist!D$2:D$150,$T4),)</f>
         <v>0</v>
       </c>
-      <c r="O4" s="16" cm="1">
+      <c r="O4" s="13" cm="1">
         <f t="array" ref="O4">IF(NOT(ISNA($T4)),INDEX(Pricelist!F$2:F$150,$T4),)</f>
         <v>0</v>
       </c>
-      <c r="P4" s="16" cm="1">
+      <c r="P4" s="13" cm="1">
         <f t="array" ref="P4">IF(NOT(ISNA($T4)),INDEX(Pricelist!G$2:G$150,$T4),)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="16" cm="1">
+      <c r="Q4" s="13" cm="1">
         <f t="array" ref="Q4">IF(NOT(ISNA($T4)),INDEX(Pricelist!H$2:H$150,$T4),)</f>
         <v>0</v>
       </c>
-      <c r="R4" s="16" cm="1">
+      <c r="R4" s="13" cm="1">
         <f t="array" ref="R4">IF(NOT(ISNA($T4)),INDEX(Pricelist!I$2:I$150,$T4),)</f>
         <v>0</v>
       </c>
@@ -3003,19 +3028,19 @@
         <f t="array" ref="N5">IF(NOT(ISNA($T5)),INDEX(Pricelist!D$2:D$150,$T5),)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="16" cm="1">
+      <c r="O5" s="13" cm="1">
         <f t="array" ref="O5">IF(NOT(ISNA($T5)),INDEX(Pricelist!F$2:F$150,$T5),)</f>
         <v>0</v>
       </c>
-      <c r="P5" s="16" cm="1">
+      <c r="P5" s="13" cm="1">
         <f t="array" ref="P5">IF(NOT(ISNA($T5)),INDEX(Pricelist!G$2:G$150,$T5),)</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="16" cm="1">
+      <c r="Q5" s="13" cm="1">
         <f t="array" ref="Q5">IF(NOT(ISNA($T5)),INDEX(Pricelist!H$2:H$150,$T5),)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="16" cm="1">
+      <c r="R5" s="13" cm="1">
         <f t="array" ref="R5">IF(NOT(ISNA($T5)),INDEX(Pricelist!I$2:I$150,$T5),)</f>
         <v>0</v>
       </c>
@@ -3071,19 +3096,19 @@
         <f t="array" ref="N6">IF(NOT(ISNA($T6)),INDEX(Pricelist!D$2:D$150,$T6),)</f>
         <v>0</v>
       </c>
-      <c r="O6" s="16" cm="1">
+      <c r="O6" s="13" cm="1">
         <f t="array" ref="O6">IF(NOT(ISNA($T6)),INDEX(Pricelist!F$2:F$150,$T6),)</f>
         <v>0</v>
       </c>
-      <c r="P6" s="16" cm="1">
+      <c r="P6" s="13" cm="1">
         <f t="array" ref="P6">IF(NOT(ISNA($T6)),INDEX(Pricelist!G$2:G$150,$T6),)</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="16" cm="1">
+      <c r="Q6" s="13" cm="1">
         <f t="array" ref="Q6">IF(NOT(ISNA($T6)),INDEX(Pricelist!H$2:H$150,$T6),)</f>
         <v>0</v>
       </c>
-      <c r="R6" s="16" cm="1">
+      <c r="R6" s="13" cm="1">
         <f t="array" ref="R6">IF(NOT(ISNA($T6)),INDEX(Pricelist!I$2:I$150,$T6),)</f>
         <v>0</v>
       </c>
@@ -3139,19 +3164,19 @@
         <f t="array" ref="N7">IF(NOT(ISNA($T7)),INDEX(Pricelist!D$2:D$150,$T7),)</f>
         <v>0</v>
       </c>
-      <c r="O7" s="16" cm="1">
+      <c r="O7" s="13" cm="1">
         <f t="array" ref="O7">IF(NOT(ISNA($T7)),INDEX(Pricelist!F$2:F$150,$T7),)</f>
         <v>0</v>
       </c>
-      <c r="P7" s="16" cm="1">
+      <c r="P7" s="13" cm="1">
         <f t="array" ref="P7">IF(NOT(ISNA($T7)),INDEX(Pricelist!G$2:G$150,$T7),)</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="16" cm="1">
+      <c r="Q7" s="13" cm="1">
         <f t="array" ref="Q7">IF(NOT(ISNA($T7)),INDEX(Pricelist!H$2:H$150,$T7),)</f>
         <v>0</v>
       </c>
-      <c r="R7" s="16" cm="1">
+      <c r="R7" s="13" cm="1">
         <f t="array" ref="R7">IF(NOT(ISNA($T7)),INDEX(Pricelist!I$2:I$150,$T7),)</f>
         <v>0</v>
       </c>
@@ -3207,19 +3232,19 @@
         <f t="array" ref="N8">IF(NOT(ISNA($T8)),INDEX(Pricelist!D$2:D$150,$T8),)</f>
         <v>0</v>
       </c>
-      <c r="O8" s="16" cm="1">
+      <c r="O8" s="13" cm="1">
         <f t="array" ref="O8">IF(NOT(ISNA($T8)),INDEX(Pricelist!F$2:F$150,$T8),)</f>
         <v>0</v>
       </c>
-      <c r="P8" s="16" cm="1">
+      <c r="P8" s="13" cm="1">
         <f t="array" ref="P8">IF(NOT(ISNA($T8)),INDEX(Pricelist!G$2:G$150,$T8),)</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="16" cm="1">
+      <c r="Q8" s="13" cm="1">
         <f t="array" ref="Q8">IF(NOT(ISNA($T8)),INDEX(Pricelist!H$2:H$150,$T8),)</f>
         <v>0</v>
       </c>
-      <c r="R8" s="16" cm="1">
+      <c r="R8" s="13" cm="1">
         <f t="array" ref="R8">IF(NOT(ISNA($T8)),INDEX(Pricelist!I$2:I$150,$T8),)</f>
         <v>0</v>
       </c>
@@ -3275,19 +3300,19 @@
         <f t="array" ref="N9">IF(NOT(ISNA($T9)),INDEX(Pricelist!D$2:D$150,$T9),)</f>
         <v>0</v>
       </c>
-      <c r="O9" s="16" cm="1">
+      <c r="O9" s="13" cm="1">
         <f t="array" ref="O9">IF(NOT(ISNA($T9)),INDEX(Pricelist!F$2:F$150,$T9),)</f>
         <v>0</v>
       </c>
-      <c r="P9" s="16" cm="1">
+      <c r="P9" s="13" cm="1">
         <f t="array" ref="P9">IF(NOT(ISNA($T9)),INDEX(Pricelist!G$2:G$150,$T9),)</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="16" cm="1">
+      <c r="Q9" s="13" cm="1">
         <f t="array" ref="Q9">IF(NOT(ISNA($T9)),INDEX(Pricelist!H$2:H$150,$T9),)</f>
         <v>0</v>
       </c>
-      <c r="R9" s="16" cm="1">
+      <c r="R9" s="13" cm="1">
         <f t="array" ref="R9">IF(NOT(ISNA($T9)),INDEX(Pricelist!I$2:I$150,$T9),)</f>
         <v>0</v>
       </c>
@@ -3343,19 +3368,19 @@
         <f t="array" ref="N10">IF(NOT(ISNA($T10)),INDEX(Pricelist!D$2:D$150,$T10),)</f>
         <v>0</v>
       </c>
-      <c r="O10" s="16" cm="1">
+      <c r="O10" s="13" cm="1">
         <f t="array" ref="O10">IF(NOT(ISNA($T10)),INDEX(Pricelist!F$2:F$150,$T10),)</f>
         <v>0</v>
       </c>
-      <c r="P10" s="16" cm="1">
+      <c r="P10" s="13" cm="1">
         <f t="array" ref="P10">IF(NOT(ISNA($T10)),INDEX(Pricelist!G$2:G$150,$T10),)</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="16" cm="1">
+      <c r="Q10" s="13" cm="1">
         <f t="array" ref="Q10">IF(NOT(ISNA($T10)),INDEX(Pricelist!H$2:H$150,$T10),)</f>
         <v>0</v>
       </c>
-      <c r="R10" s="16" cm="1">
+      <c r="R10" s="13" cm="1">
         <f t="array" ref="R10">IF(NOT(ISNA($T10)),INDEX(Pricelist!I$2:I$150,$T10),)</f>
         <v>0</v>
       </c>
@@ -3411,19 +3436,19 @@
         <f t="array" ref="N11">IF(NOT(ISNA($T11)),INDEX(Pricelist!D$2:D$150,$T11),)</f>
         <v>0</v>
       </c>
-      <c r="O11" s="16" cm="1">
+      <c r="O11" s="13" cm="1">
         <f t="array" ref="O11">IF(NOT(ISNA($T11)),INDEX(Pricelist!F$2:F$150,$T11),)</f>
         <v>0</v>
       </c>
-      <c r="P11" s="16" cm="1">
+      <c r="P11" s="13" cm="1">
         <f t="array" ref="P11">IF(NOT(ISNA($T11)),INDEX(Pricelist!G$2:G$150,$T11),)</f>
         <v>0</v>
       </c>
-      <c r="Q11" s="16" cm="1">
+      <c r="Q11" s="13" cm="1">
         <f t="array" ref="Q11">IF(NOT(ISNA($T11)),INDEX(Pricelist!H$2:H$150,$T11),)</f>
         <v>0</v>
       </c>
-      <c r="R11" s="16" cm="1">
+      <c r="R11" s="13" cm="1">
         <f t="array" ref="R11">IF(NOT(ISNA($T11)),INDEX(Pricelist!I$2:I$150,$T11),)</f>
         <v>0</v>
       </c>
@@ -3479,19 +3504,19 @@
         <f t="array" ref="N12">IF(NOT(ISNA($T12)),INDEX(Pricelist!D$2:D$150,$T12),)</f>
         <v>0</v>
       </c>
-      <c r="O12" s="16" cm="1">
+      <c r="O12" s="13" cm="1">
         <f t="array" ref="O12">IF(NOT(ISNA($T12)),INDEX(Pricelist!F$2:F$150,$T12),)</f>
         <v>0</v>
       </c>
-      <c r="P12" s="16" cm="1">
+      <c r="P12" s="13" cm="1">
         <f t="array" ref="P12">IF(NOT(ISNA($T12)),INDEX(Pricelist!G$2:G$150,$T12),)</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="16" cm="1">
+      <c r="Q12" s="13" cm="1">
         <f t="array" ref="Q12">IF(NOT(ISNA($T12)),INDEX(Pricelist!H$2:H$150,$T12),)</f>
         <v>0</v>
       </c>
-      <c r="R12" s="16" cm="1">
+      <c r="R12" s="13" cm="1">
         <f t="array" ref="R12">IF(NOT(ISNA($T12)),INDEX(Pricelist!I$2:I$150,$T12),)</f>
         <v>0</v>
       </c>
@@ -3537,19 +3562,19 @@
         <f t="array" ref="N13">IF(NOT(ISNA($T13)),INDEX(Pricelist!D$2:D$150,$T13),)</f>
         <v>0</v>
       </c>
-      <c r="O13" s="16" cm="1">
+      <c r="O13" s="13" cm="1">
         <f t="array" ref="O13">IF(NOT(ISNA($T13)),INDEX(Pricelist!F$2:F$150,$T13),)</f>
         <v>0</v>
       </c>
-      <c r="P13" s="16" cm="1">
+      <c r="P13" s="13" cm="1">
         <f t="array" ref="P13">IF(NOT(ISNA($T13)),INDEX(Pricelist!G$2:G$150,$T13),)</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="16" cm="1">
+      <c r="Q13" s="13" cm="1">
         <f t="array" ref="Q13">IF(NOT(ISNA($T13)),INDEX(Pricelist!H$2:H$150,$T13),)</f>
         <v>0</v>
       </c>
-      <c r="R13" s="16" cm="1">
+      <c r="R13" s="13" cm="1">
         <f t="array" ref="R13">IF(NOT(ISNA($T13)),INDEX(Pricelist!I$2:I$150,$T13),)</f>
         <v>0</v>
       </c>
@@ -3595,19 +3620,19 @@
         <f t="array" ref="N14">IF(NOT(ISNA($T14)),INDEX(Pricelist!D$2:D$150,$T14),)</f>
         <v>0</v>
       </c>
-      <c r="O14" s="16" cm="1">
+      <c r="O14" s="13" cm="1">
         <f t="array" ref="O14">IF(NOT(ISNA($T14)),INDEX(Pricelist!F$2:F$150,$T14),)</f>
         <v>0</v>
       </c>
-      <c r="P14" s="16" cm="1">
+      <c r="P14" s="13" cm="1">
         <f t="array" ref="P14">IF(NOT(ISNA($T14)),INDEX(Pricelist!G$2:G$150,$T14),)</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="16" cm="1">
+      <c r="Q14" s="13" cm="1">
         <f t="array" ref="Q14">IF(NOT(ISNA($T14)),INDEX(Pricelist!H$2:H$150,$T14),)</f>
         <v>0</v>
       </c>
-      <c r="R14" s="16" cm="1">
+      <c r="R14" s="13" cm="1">
         <f t="array" ref="R14">IF(NOT(ISNA($T14)),INDEX(Pricelist!I$2:I$150,$T14),)</f>
         <v>0</v>
       </c>
@@ -3653,19 +3678,19 @@
         <f t="array" ref="N15">IF(NOT(ISNA($T15)),INDEX(Pricelist!D$2:D$150,$T15),)</f>
         <v>0</v>
       </c>
-      <c r="O15" s="16" cm="1">
+      <c r="O15" s="13" cm="1">
         <f t="array" ref="O15">IF(NOT(ISNA($T15)),INDEX(Pricelist!F$2:F$150,$T15),)</f>
         <v>0</v>
       </c>
-      <c r="P15" s="16" cm="1">
+      <c r="P15" s="13" cm="1">
         <f t="array" ref="P15">IF(NOT(ISNA($T15)),INDEX(Pricelist!G$2:G$150,$T15),)</f>
         <v>0</v>
       </c>
-      <c r="Q15" s="16" cm="1">
+      <c r="Q15" s="13" cm="1">
         <f t="array" ref="Q15">IF(NOT(ISNA($T15)),INDEX(Pricelist!H$2:H$150,$T15),)</f>
         <v>0</v>
       </c>
-      <c r="R15" s="16" cm="1">
+      <c r="R15" s="13" cm="1">
         <f t="array" ref="R15">IF(NOT(ISNA($T15)),INDEX(Pricelist!I$2:I$150,$T15),)</f>
         <v>0</v>
       </c>
@@ -3711,19 +3736,19 @@
         <f t="array" ref="N16">IF(NOT(ISNA($T16)),INDEX(Pricelist!D$2:D$150,$T16),)</f>
         <v>0</v>
       </c>
-      <c r="O16" s="16" cm="1">
+      <c r="O16" s="13" cm="1">
         <f t="array" ref="O16">IF(NOT(ISNA($T16)),INDEX(Pricelist!F$2:F$150,$T16),)</f>
         <v>0</v>
       </c>
-      <c r="P16" s="16" cm="1">
+      <c r="P16" s="13" cm="1">
         <f t="array" ref="P16">IF(NOT(ISNA($T16)),INDEX(Pricelist!G$2:G$150,$T16),)</f>
         <v>0</v>
       </c>
-      <c r="Q16" s="16" cm="1">
+      <c r="Q16" s="13" cm="1">
         <f t="array" ref="Q16">IF(NOT(ISNA($T16)),INDEX(Pricelist!H$2:H$150,$T16),)</f>
         <v>0</v>
       </c>
-      <c r="R16" s="16" cm="1">
+      <c r="R16" s="13" cm="1">
         <f t="array" ref="R16">IF(NOT(ISNA($T16)),INDEX(Pricelist!I$2:I$150,$T16),)</f>
         <v>0</v>
       </c>
@@ -3769,19 +3794,19 @@
         <f t="array" ref="N17">IF(NOT(ISNA($T17)),INDEX(Pricelist!D$2:D$150,$T17),)</f>
         <v>0</v>
       </c>
-      <c r="O17" s="16" cm="1">
+      <c r="O17" s="13" cm="1">
         <f t="array" ref="O17">IF(NOT(ISNA($T17)),INDEX(Pricelist!F$2:F$150,$T17),)</f>
         <v>0</v>
       </c>
-      <c r="P17" s="16" cm="1">
+      <c r="P17" s="13" cm="1">
         <f t="array" ref="P17">IF(NOT(ISNA($T17)),INDEX(Pricelist!G$2:G$150,$T17),)</f>
         <v>0</v>
       </c>
-      <c r="Q17" s="16" cm="1">
+      <c r="Q17" s="13" cm="1">
         <f t="array" ref="Q17">IF(NOT(ISNA($T17)),INDEX(Pricelist!H$2:H$150,$T17),)</f>
         <v>0</v>
       </c>
-      <c r="R17" s="16" cm="1">
+      <c r="R17" s="13" cm="1">
         <f t="array" ref="R17">IF(NOT(ISNA($T17)),INDEX(Pricelist!I$2:I$150,$T17),)</f>
         <v>0</v>
       </c>
@@ -3827,19 +3852,19 @@
         <f t="array" ref="N18">IF(NOT(ISNA($T18)),INDEX(Pricelist!D$2:D$150,$T18),)</f>
         <v>0</v>
       </c>
-      <c r="O18" s="16" cm="1">
+      <c r="O18" s="13" cm="1">
         <f t="array" ref="O18">IF(NOT(ISNA($T18)),INDEX(Pricelist!F$2:F$150,$T18),)</f>
         <v>0</v>
       </c>
-      <c r="P18" s="16" cm="1">
+      <c r="P18" s="13" cm="1">
         <f t="array" ref="P18">IF(NOT(ISNA($T18)),INDEX(Pricelist!G$2:G$150,$T18),)</f>
         <v>0</v>
       </c>
-      <c r="Q18" s="16" cm="1">
+      <c r="Q18" s="13" cm="1">
         <f t="array" ref="Q18">IF(NOT(ISNA($T18)),INDEX(Pricelist!H$2:H$150,$T18),)</f>
         <v>0</v>
       </c>
-      <c r="R18" s="16" cm="1">
+      <c r="R18" s="13" cm="1">
         <f t="array" ref="R18">IF(NOT(ISNA($T18)),INDEX(Pricelist!I$2:I$150,$T18),)</f>
         <v>0</v>
       </c>
@@ -3885,19 +3910,19 @@
         <f t="array" ref="N19">IF(NOT(ISNA($T19)),INDEX(Pricelist!D$2:D$150,$T19),)</f>
         <v>0</v>
       </c>
-      <c r="O19" s="16" cm="1">
+      <c r="O19" s="13" cm="1">
         <f t="array" ref="O19">IF(NOT(ISNA($T19)),INDEX(Pricelist!F$2:F$150,$T19),)</f>
         <v>0</v>
       </c>
-      <c r="P19" s="16" cm="1">
+      <c r="P19" s="13" cm="1">
         <f t="array" ref="P19">IF(NOT(ISNA($T19)),INDEX(Pricelist!G$2:G$150,$T19),)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="16" cm="1">
+      <c r="Q19" s="13" cm="1">
         <f t="array" ref="Q19">IF(NOT(ISNA($T19)),INDEX(Pricelist!H$2:H$150,$T19),)</f>
         <v>0</v>
       </c>
-      <c r="R19" s="16" cm="1">
+      <c r="R19" s="13" cm="1">
         <f t="array" ref="R19">IF(NOT(ISNA($T19)),INDEX(Pricelist!I$2:I$150,$T19),)</f>
         <v>0</v>
       </c>
@@ -3943,19 +3968,19 @@
         <f t="array" ref="N20">IF(NOT(ISNA($T20)),INDEX(Pricelist!D$2:D$150,$T20),)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="16" cm="1">
+      <c r="O20" s="13" cm="1">
         <f t="array" ref="O20">IF(NOT(ISNA($T20)),INDEX(Pricelist!F$2:F$150,$T20),)</f>
         <v>0</v>
       </c>
-      <c r="P20" s="16" cm="1">
+      <c r="P20" s="13" cm="1">
         <f t="array" ref="P20">IF(NOT(ISNA($T20)),INDEX(Pricelist!G$2:G$150,$T20),)</f>
         <v>0</v>
       </c>
-      <c r="Q20" s="16" cm="1">
+      <c r="Q20" s="13" cm="1">
         <f t="array" ref="Q20">IF(NOT(ISNA($T20)),INDEX(Pricelist!H$2:H$150,$T20),)</f>
         <v>0</v>
       </c>
-      <c r="R20" s="16" cm="1">
+      <c r="R20" s="13" cm="1">
         <f t="array" ref="R20">IF(NOT(ISNA($T20)),INDEX(Pricelist!I$2:I$150,$T20),)</f>
         <v>0</v>
       </c>
@@ -4001,19 +4026,19 @@
         <f t="array" ref="N21">IF(NOT(ISNA($T21)),INDEX(Pricelist!D$2:D$150,$T21),)</f>
         <v>0</v>
       </c>
-      <c r="O21" s="16" cm="1">
+      <c r="O21" s="13" cm="1">
         <f t="array" ref="O21">IF(NOT(ISNA($T21)),INDEX(Pricelist!F$2:F$150,$T21),)</f>
         <v>0</v>
       </c>
-      <c r="P21" s="16" cm="1">
+      <c r="P21" s="13" cm="1">
         <f t="array" ref="P21">IF(NOT(ISNA($T21)),INDEX(Pricelist!G$2:G$150,$T21),)</f>
         <v>0</v>
       </c>
-      <c r="Q21" s="16" cm="1">
+      <c r="Q21" s="13" cm="1">
         <f t="array" ref="Q21">IF(NOT(ISNA($T21)),INDEX(Pricelist!H$2:H$150,$T21),)</f>
         <v>0</v>
       </c>
-      <c r="R21" s="16" cm="1">
+      <c r="R21" s="13" cm="1">
         <f t="array" ref="R21">IF(NOT(ISNA($T21)),INDEX(Pricelist!I$2:I$150,$T21),)</f>
         <v>0</v>
       </c>
@@ -4059,19 +4084,19 @@
         <f t="array" ref="N22">IF(NOT(ISNA($T22)),INDEX(Pricelist!D$2:D$150,$T22),)</f>
         <v>0</v>
       </c>
-      <c r="O22" s="16" cm="1">
+      <c r="O22" s="13" cm="1">
         <f t="array" ref="O22">IF(NOT(ISNA($T22)),INDEX(Pricelist!F$2:F$150,$T22),)</f>
         <v>0</v>
       </c>
-      <c r="P22" s="16" cm="1">
+      <c r="P22" s="13" cm="1">
         <f t="array" ref="P22">IF(NOT(ISNA($T22)),INDEX(Pricelist!G$2:G$150,$T22),)</f>
         <v>0</v>
       </c>
-      <c r="Q22" s="16" cm="1">
+      <c r="Q22" s="13" cm="1">
         <f t="array" ref="Q22">IF(NOT(ISNA($T22)),INDEX(Pricelist!H$2:H$150,$T22),)</f>
         <v>0</v>
       </c>
-      <c r="R22" s="16" cm="1">
+      <c r="R22" s="13" cm="1">
         <f t="array" ref="R22">IF(NOT(ISNA($T22)),INDEX(Pricelist!I$2:I$150,$T22),)</f>
         <v>0</v>
       </c>
@@ -4117,19 +4142,19 @@
         <f t="array" ref="N23">IF(NOT(ISNA($T23)),INDEX(Pricelist!D$2:D$150,$T23),)</f>
         <v>0</v>
       </c>
-      <c r="O23" s="16" cm="1">
+      <c r="O23" s="13" cm="1">
         <f t="array" ref="O23">IF(NOT(ISNA($T23)),INDEX(Pricelist!F$2:F$150,$T23),)</f>
         <v>0</v>
       </c>
-      <c r="P23" s="16" cm="1">
+      <c r="P23" s="13" cm="1">
         <f t="array" ref="P23">IF(NOT(ISNA($T23)),INDEX(Pricelist!G$2:G$150,$T23),)</f>
         <v>0</v>
       </c>
-      <c r="Q23" s="16" cm="1">
+      <c r="Q23" s="13" cm="1">
         <f t="array" ref="Q23">IF(NOT(ISNA($T23)),INDEX(Pricelist!H$2:H$150,$T23),)</f>
         <v>0</v>
       </c>
-      <c r="R23" s="16" cm="1">
+      <c r="R23" s="13" cm="1">
         <f t="array" ref="R23">IF(NOT(ISNA($T23)),INDEX(Pricelist!I$2:I$150,$T23),)</f>
         <v>0</v>
       </c>

</xml_diff>